<commit_message>
New datasheets and simulations added. Target is to improve the power of the booster circuit of the diver flasher.
</commit_message>
<xml_diff>
--- a/documents/Berechnungen, Bauteile & Bestellliste.xlsx
+++ b/documents/Berechnungen, Bauteile & Bestellliste.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\_Eggeling_Engineering\Projekte\Eggeling\3_Tauchen_&amp;_Sport\Einfacher LED-Blitzer\V2\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_EinfacherLEDBlitzer(GH)\diver_led_tools\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD978134-0922-4B90-9818-F6608BA86161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C0A386-A616-4C95-8E56-5916F274A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="581" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bestelliste" sheetId="1" r:id="rId1"/>
     <sheet name="Flasher" sheetId="6" r:id="rId2"/>
-    <sheet name="Batterien &amp; Akkus" sheetId="5" r:id="rId3"/>
-    <sheet name="LEDs" sheetId="4" r:id="rId4"/>
-    <sheet name="Prüfung Bauteilgrößen" sheetId="3" r:id="rId5"/>
-    <sheet name="Nebenrechnungen" sheetId="2" r:id="rId6"/>
+    <sheet name="Transistoren" sheetId="8" r:id="rId3"/>
+    <sheet name="Batterien &amp; Akkus" sheetId="5" r:id="rId4"/>
+    <sheet name="LEDs" sheetId="4" r:id="rId5"/>
+    <sheet name="wo Booster" sheetId="10" r:id="rId6"/>
+    <sheet name="Prüfung Bauteilgrößen" sheetId="3" r:id="rId7"/>
+    <sheet name="Nebenrechnungen" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="275">
   <si>
     <t>Komponente</t>
   </si>
@@ -251,9 +253,6 @@
   </si>
   <si>
     <t>LB-P200B2C-H</t>
-  </si>
-  <si>
-    <t>Diver Marker</t>
   </si>
   <si>
     <t>LB-P200G3C-H</t>
@@ -387,9 +386,6 @@
   </si>
   <si>
     <t xml:space="preserve">Beide sind in etwas gleich groß, aber unterschiedlich dick! </t>
-  </si>
-  <si>
-    <t>Leistung Vorwiderstand LED (Blitzer)</t>
   </si>
   <si>
     <t>Abhängigkeit Widerstand / Strom</t>
@@ -718,6 +714,180 @@
   </si>
   <si>
     <t>PIC16LF15313</t>
+  </si>
+  <si>
+    <t>Diver marker</t>
+  </si>
+  <si>
+    <t>Diver flasher</t>
+  </si>
+  <si>
+    <t>Leistung Vorwiderstand LED Flasher</t>
+  </si>
+  <si>
+    <t>Optimierungsansatz ohne Flasher</t>
+  </si>
+  <si>
+    <t>Betrachtungen Spannungsverlust Schalttransistor</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>MJD122T4 (PCB)</t>
+  </si>
+  <si>
+    <t>2N6386 (PB 1)</t>
+  </si>
+  <si>
+    <t>IRF540N (PB 2)</t>
+  </si>
+  <si>
+    <t>UCE , bzw. UDS [V]</t>
+  </si>
+  <si>
+    <t>DMT8008LFG</t>
+  </si>
+  <si>
+    <t>Mouser Nummer</t>
+  </si>
+  <si>
+    <t>621-DMT8008LFG-7</t>
+  </si>
+  <si>
+    <t>Mögliche Typen</t>
+  </si>
+  <si>
+    <t>Hersteller</t>
+  </si>
+  <si>
+    <t>Umax</t>
+  </si>
+  <si>
+    <t>RDSOn</t>
+  </si>
+  <si>
+    <t>Imax</t>
+  </si>
+  <si>
+    <t>38A</t>
+  </si>
+  <si>
+    <t>80V</t>
+  </si>
+  <si>
+    <t>10mOhm
+@4,5V VGS</t>
+  </si>
+  <si>
+    <t>Gehäuse</t>
+  </si>
+  <si>
+    <t>PowerDI®3333-8</t>
+  </si>
+  <si>
+    <t>RFD16N05LSM</t>
+  </si>
+  <si>
+    <t>16A</t>
+  </si>
+  <si>
+    <t>47mOhm
+@</t>
+  </si>
+  <si>
+    <t>DPAK-2
+(TO−252AA)</t>
+  </si>
+  <si>
+    <t>Onsemi</t>
+  </si>
+  <si>
+    <t>50V</t>
+  </si>
+  <si>
+    <t>512-RFD16N05LSM9A</t>
+  </si>
+  <si>
+    <t>Opt VGS</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>20A</t>
+  </si>
+  <si>
+    <t>52mOhm
+@</t>
+  </si>
+  <si>
+    <t>HUF76629D3ST-F085</t>
+  </si>
+  <si>
+    <t>512-HUF76629D3ST</t>
+  </si>
+  <si>
+    <t>s.u</t>
+  </si>
+  <si>
+    <t>Diodes
+Incorporated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-NDB5060L </t>
+  </si>
+  <si>
+    <t>60V</t>
+  </si>
+  <si>
+    <t>26A</t>
+  </si>
+  <si>
+    <t>NDB5060L</t>
+  </si>
+  <si>
+    <t>70mOhm
+@3,3V</t>
+  </si>
+  <si>
+    <t>=&gt; Es darf kein Bipolartransistor verwendet werden!</t>
+  </si>
+  <si>
+    <t>s.u.r.</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>LED Spannung @750mA</t>
+  </si>
+  <si>
+    <t>=&gt; Ein stabiler Betrieb ist ohne Booster nicht möglich</t>
+  </si>
+  <si>
+    <t>Umax bei Ladestand 100%</t>
+  </si>
+  <si>
+    <t>Umin @ Ladestand 20%</t>
+  </si>
+  <si>
+    <t>Batteriespannung @0,5C *</t>
+  </si>
+  <si>
+    <t>*0,5 C, da Kapazität 2,6Ah und Entladestrom ca. 1,5A</t>
+  </si>
+  <si>
+    <t>Actung: UCE bis zu 2V =&gt; Strom nicht reproduzierbar!</t>
+  </si>
+  <si>
+    <t>Siehe dazu auch Tab "Transistoren"</t>
   </si>
 </sst>
 </file>
@@ -729,7 +899,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -795,8 +965,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -828,8 +1028,20 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -885,8 +1097,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -895,8 +1127,11 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -967,6 +1202,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -991,19 +1229,46 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="0" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="10"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="10" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="11">
     <cellStyle name="Berechnung" xfId="5" builtinId="22"/>
     <cellStyle name="Eingabe" xfId="4" builtinId="20"/>
+    <cellStyle name="Ergebnis" xfId="10" builtinId="25"/>
     <cellStyle name="Gut" xfId="2" builtinId="26"/>
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="3" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="8" builtinId="15"/>
     <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Überschrift 2" xfId="9" builtinId="17"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2315,16 +2580,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>47442</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85542</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>400502</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2354,8 +2619,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5673542" y="5765800"/>
-          <a:ext cx="1216208" cy="1473200"/>
+          <a:off x="5978342" y="5740400"/>
+          <a:ext cx="943610" cy="1143000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2376,60 +2641,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>192658</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>99466</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>85652</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>179236</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Grafik 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5693E8E1-542F-AFE2-79AE-470BB755E6C4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="6928268">
-          <a:off x="5620595" y="7708079"/>
-          <a:ext cx="1184670" cy="788344"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>81338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>548802</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>168188</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2445,7 +2666,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2453,7 +2674,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7162800" y="5834438"/>
-          <a:ext cx="6397152" cy="1480762"/>
+          <a:ext cx="5422900" cy="1255250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2466,6 +2687,99 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1028699</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>622298</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12624B70-5EEE-62BC-D795-41CB827DEC5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10725149" y="2082801"/>
+          <a:ext cx="4349749" cy="3568699"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>144244</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>459914</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBEA9DF6-2B5B-CBCA-A03B-59C0371FA725}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="387350" y="2284194"/>
+          <a:ext cx="8949864" cy="3818156"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2826,27 +3140,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>152005</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>127001</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>164596</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1">
+        <xdr:cNvPr id="3" name="Grafik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A488B5-C522-973C-0FFF-A8CE1D06D8E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5EC2D89-B7A5-922B-8C4A-7EC1AF54E51D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2862,8 +3176,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1" y="1"/>
-          <a:ext cx="9296004" cy="2520950"/>
+          <a:off x="57150" y="476250"/>
+          <a:ext cx="10013446" cy="4343400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2875,22 +3189,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>275370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>107446</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>165623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2">
+        <xdr:cNvPr id="4" name="Grafik 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5EC2D89-B7A5-922B-8C4A-7EC1AF54E51D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5490DAD4-E157-2800-A5EA-42F5E2685A7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2906,8 +3220,449 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2692400"/>
-          <a:ext cx="10013446" cy="4343400"/>
+          <a:off x="12700" y="5177570"/>
+          <a:ext cx="9721850" cy="2398503"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>685440</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>146140</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Freihand 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFA853C8-4421-090E-B8AC-DC39028CCEA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2971440" y="3244650"/>
+            <a:ext cx="1047960" cy="32040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Freihand 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFA853C8-4421-090E-B8AC-DC39028CCEA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2917800" y="3137010"/>
+              <a:ext cx="1155600" cy="247680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>685440</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="8" name="Freihand 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9245D2E3-D71B-44D9-B826-A87A82F57DDB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2971440" y="5473410"/>
+            <a:ext cx="1105200" cy="32040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Freihand 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9245D2E3-D71B-44D9-B826-A87A82F57DDB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2917800" y="5365410"/>
+              <a:ext cx="1212840" cy="247680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>734717</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>171968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Grafik 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BF28138-245E-B5FB-9784-0E6FE9E9245C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7581900"/>
+          <a:ext cx="9878717" cy="2394468"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>761760</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>126840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>686040</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>158880</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="14" name="Freihand 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D55566-E139-81AF-EBCD-08732221FA7E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3047760" y="8089740"/>
+            <a:ext cx="1448280" cy="32040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="14" name="Freihand 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D55566-E139-81AF-EBCD-08732221FA7E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2993760" y="7982100"/>
+              <a:ext cx="1555920" cy="247680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>284017</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Grafik 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C968A350-8DC9-48CA-AA1D-FA73B8C0D2BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9931400" y="5391150"/>
+          <a:ext cx="5592617" cy="2184400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>399720</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>183860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>89160</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>6550</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="17" name="Freihand 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5155698D-C875-1FA7-A3D9-909FBF6F307F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="12591720" y="7226010"/>
+            <a:ext cx="2737440" cy="6840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="17" name="Freihand 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5155698D-C875-1FA7-A3D9-909FBF6F307F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12537720" y="7118010"/>
+              <a:ext cx="2845080" cy="222480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>679449</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>502852</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D95770-985A-4436-AB5D-39E04F0AB2C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4616449" y="209550"/>
+          <a:ext cx="4395403" cy="3365500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>302765</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>582712</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D771E373-8A9A-C6F0-6AA6-0DF58893490F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="302765" y="2527300"/>
+          <a:ext cx="4216947" cy="1060450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2917,6 +3672,179 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>431404</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD1404F4-FB76-4D16-B79A-CD5865C0296F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1670050"/>
+          <a:ext cx="9296004" cy="2520950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-01-03T19:31:44.328"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.3" units="cm"/>
+      <inkml:brushProperty name="height" value="0.6" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFC00"/>
+      <inkml:brushProperty name="tip" value="rectangle"/>
+      <inkml:brushProperty name="rasterOp" value="maskPen"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 0,'2910'88'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-01-03T19:31:46.944"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.3" units="cm"/>
+      <inkml:brushProperty name="height" value="0.6" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFC00"/>
+      <inkml:brushProperty name="tip" value="rectangle"/>
+      <inkml:brushProperty name="rasterOp" value="maskPen"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 88 0,'3069'-88'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-01-03T19:34:22.185"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.3" units="cm"/>
+      <inkml:brushProperty name="height" value="0.6" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFC00"/>
+      <inkml:brushProperty name="tip" value="rectangle"/>
+      <inkml:brushProperty name="rasterOp" value="maskPen"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 89 0,'4022'-88'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-01-03T22:10:37.631"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.3" units="cm"/>
+      <inkml:brushProperty name="height" value="0.6" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFC00"/>
+      <inkml:brushProperty name="tip" value="rectangle"/>
+      <inkml:brushProperty name="rasterOp" value="maskPen"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 18 0,'7603'-18'0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3255,7 +4183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:H15"/>
     </sheetView>
   </sheetViews>
@@ -3276,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3299,7 +4227,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -3325,7 +4253,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -3351,13 +4279,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
@@ -3377,19 +4305,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F6" s="2">
         <v>3.5</v>
@@ -3398,7 +4326,7 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -3406,7 +4334,7 @@
         <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>66</v>
@@ -3429,19 +4357,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="2">
         <v>0.46</v>
@@ -3452,19 +4380,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" s="2">
         <v>1.1000000000000001</v>
@@ -3473,18 +4401,18 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>14</v>
@@ -3499,24 +4427,24 @@
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="2">
         <v>0.95</v>
@@ -3525,24 +4453,24 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="2">
         <v>0.09</v>
@@ -3551,18 +4479,18 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>14</v>
@@ -3582,25 +4510,25 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>218</v>
+        <v>215</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -3608,16 +4536,16 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F15" s="2">
         <v>4.99</v>
@@ -3626,7 +4554,7 @@
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -3641,10 +4569,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
         <v>94</v>
-      </c>
-      <c r="B17" t="s">
-        <v>95</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -3653,7 +4581,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H17" t="s">
         <v>11</v>
@@ -3661,7 +4589,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3675,10 +4603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457480F2-2497-42BF-A03F-78F1F2D39AE9}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3696,60 +4624,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="A3" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:11" s="16" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C4" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>176</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>178</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="K4" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="J4" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="36">
+      <c r="A5" s="37">
         <v>3</v>
       </c>
       <c r="B5" s="23">
@@ -3781,7 +4709,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="23">
         <v>4.5</v>
       </c>
@@ -3811,7 +4739,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="23">
         <v>5</v>
       </c>
@@ -3841,7 +4769,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="23">
         <v>5.5</v>
       </c>
@@ -3871,7 +4799,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="36">
+      <c r="A9" s="37">
         <v>2</v>
       </c>
       <c r="B9" s="23">
@@ -3891,7 +4819,7 @@
       <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="23">
         <v>4.5</v>
       </c>
@@ -3909,7 +4837,7 @@
       <c r="F10" s="25"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="23">
         <v>5</v>
       </c>
@@ -3927,7 +4855,7 @@
       <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="23">
         <v>5.5</v>
       </c>
@@ -3945,7 +4873,7 @@
       <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="36">
+      <c r="A13" s="37">
         <v>1</v>
       </c>
       <c r="B13" s="23">
@@ -3965,7 +4893,7 @@
       <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="23">
         <v>4.5</v>
       </c>
@@ -3983,7 +4911,7 @@
       <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="36"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="29">
         <v>5</v>
       </c>
@@ -3999,11 +4927,11 @@
         <v>2.8287999999999998</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="23">
         <v>5.5</v>
       </c>
@@ -4019,34 +4947,34 @@
         <v>4.1139999999999999</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
+      <c r="A18" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="1:6" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C19" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>176</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>178</v>
       </c>
       <c r="F19" s="22" t="s">
         <v>6</v>
@@ -4071,83 +4999,100 @@
         <v>3.1279999999999997</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
+      <c r="A25" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>208</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>209</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="B29" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>212</v>
-      </c>
       <c r="E29" s="18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>214</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+    </row>
+    <row r="32" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
@@ -4188,11 +5133,10 @@
     <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A1:F1"/>
@@ -4214,11 +5158,247 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67B40DA-7A8A-49B4-9489-E515C1B8CB19}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7265625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F2" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="K2" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="N2" s="48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M3" t="s">
+        <v>232</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L4" t="s">
+        <v>247</v>
+      </c>
+      <c r="M4" t="s">
+        <v>249</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" t="s">
+        <v>210</v>
+      </c>
+      <c r="H5" t="s">
+        <v>252</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J5" t="s">
+        <v>264</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L5" t="s">
+        <v>247</v>
+      </c>
+      <c r="M5" t="s">
+        <v>255</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="C6" s="43">
+        <v>2</v>
+      </c>
+      <c r="D6" s="44">
+        <f>0.052*2</f>
+        <v>0.104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>261</v>
+      </c>
+      <c r="G6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H6" t="s">
+        <v>260</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J6" t="s">
+        <v>256</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L6" t="s">
+        <v>247</v>
+      </c>
+      <c r="M6" t="s">
+        <v>258</v>
+      </c>
+      <c r="N6" s="3">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="49" t="s">
+        <v>263</v>
+      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31109754-0340-407A-9A46-A4EA23310DEB}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4231,49 +5411,49 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" t="s">
         <v>103</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>104</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
         <v>108</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>109</v>
-      </c>
-      <c r="D34" t="s">
-        <v>110</v>
       </c>
       <c r="E34">
         <v>1800</v>
@@ -4282,18 +5462,18 @@
         <v>13</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" t="s">
         <v>109</v>
-      </c>
-      <c r="D35" t="s">
-        <v>110</v>
       </c>
       <c r="E35">
         <v>1100</v>
@@ -4302,7 +5482,7 @@
         <v>10.99</v>
       </c>
       <c r="H35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -4319,19 +5499,19 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F40" s="3"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
         <v>3</v>
@@ -4340,7 +5520,7 @@
         <v>4</v>
       </c>
       <c r="F56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G56" t="s">
         <v>6</v>
@@ -4348,16 +5528,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B57" t="s">
         <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E57" s="3">
         <v>3.7</v>
@@ -4366,21 +5546,21 @@
         <v>750</v>
       </c>
       <c r="G57" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E58" s="3">
         <v>4.5</v>
@@ -4389,21 +5569,21 @@
         <v>950</v>
       </c>
       <c r="G58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B59" t="s">
         <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E59" s="3">
         <v>2.0499999999999998</v>
@@ -4412,21 +5592,21 @@
         <v>1430</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E60" s="14">
         <v>2.5</v>
@@ -4435,7 +5615,7 @@
         <v>2700</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -4475,27 +5655,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE11DE5C-E2F5-436C-AB86-81BF82F258AF}">
-  <dimension ref="B41:D42"/>
+  <dimension ref="A2:A27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:F44"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>71</v>
+    <row r="2" spans="1:1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="41" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="41" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4504,12 +5681,128 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C15D1FA-A3D9-41F1-ABE3-824794C450AE}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="3.26953125" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="54">
+        <v>4</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+    </row>
+    <row r="5" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="54">
+        <v>3.6</v>
+      </c>
+      <c r="C6" s="51"/>
+      <c r="D6" s="52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="51">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="55" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A12:F12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE47ED3-E916-475E-B2EE-F7B7619CA98E}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4639,727 +5932,731 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922524F8-C67C-466F-AC41-92FE358F9A73}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.08984375" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" customWidth="1"/>
-    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.7265625" customWidth="1"/>
-    <col min="15" max="15" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7265625" customWidth="1"/>
+    <col min="12" max="12" width="25.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="H1" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="E1" s="32" t="s">
+      <c r="C2" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="E2" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5">
+        <v>18650</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2600</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.124</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="9">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="I5" s="8">
+        <v>50</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="8">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="8">
+        <f>I3*I6/100</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="H8" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I8" s="8">
+        <f>I7/0.8</f>
+        <v>9.3749999999999986E-2</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="5">
+        <v>18650</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2600</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="5">
+        <v>17500</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1100</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="9">
+        <f>I8+I9</f>
+        <v>0.12374999999999999</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C11" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" s="9">
+        <f>I10*1</f>
+        <v>0.12374999999999999</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="12">
+        <f>I2/(I11*1000)</f>
+        <v>21.010101010101014</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="9">
+        <f>(C11*C12/100)+C13</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="9">
+        <f>C14*1</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="12">
+        <f>C9/(C15*1000)</f>
+        <v>162.5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B17" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="12">
+        <f>C10/(C15*1000)</f>
+        <v>68.75</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B18" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="20" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="H20" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="8">
+        <v>950</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B22" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1430</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" t="s">
+        <v>154</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6">
+      <c r="I22" s="6">
         <v>0.33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J22" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8">
-        <v>0.33</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H3" s="5" t="s">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2750</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="F23" t="s">
+        <v>161</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B24" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" t="s">
+        <v>146</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="6">
+        <v>50</v>
+      </c>
+      <c r="J24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="8">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="H25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0.124</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="6">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="8">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="9">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="8">
-        <v>3</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0.06</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="F26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6">
+      <c r="I26" s="6">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="J26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="7">
-        <f>B4*B7/100</f>
+      <c r="C27" s="9">
+        <f>(C24*C25/100)+C26</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="7">
+        <f>I23*I26/100</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="J27" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="K8" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B28" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="9">
+        <f>C27*1</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="7">
-        <f>B8*B8*B3</f>
+      <c r="I28" s="7">
+        <f>I27*I27*I22</f>
         <v>7.4250000000000002E-5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="J28" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="5">
-        <v>18650</v>
-      </c>
-      <c r="F9" s="8">
-        <v>2600</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="K9" s="5">
-        <v>18650</v>
-      </c>
-      <c r="L9" s="8">
-        <v>2600</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="12">
+        <f>C21/(C28*1000)</f>
+        <v>54.285714285714285</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" t="s">
+        <v>144</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="7">
-        <f>B4*B4*B3</f>
+      <c r="I29" s="7">
+        <f>I23*I23*I22</f>
         <v>2.9700000000000001E-2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="J29" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="5">
-        <v>17500</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1100</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="L10" s="8">
-        <v>2</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="12">
+        <f>C22/(C28*1000)</f>
+        <v>81.714285714285708</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" t="s">
+        <v>153</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11">
+      <c r="I30">
         <v>0.15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="J30" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.12</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" t="s">
-        <v>148</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="L11" s="8">
-        <v>2</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="N11" s="5"/>
-      <c r="O11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="12">
+        <f>C23/(C28*1000)</f>
+        <v>157.14285714285714</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" t="s">
+        <v>160</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="I31">
         <v>0.1</v>
       </c>
-      <c r="C12" t="s">
+      <c r="J31" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="8">
-        <v>5</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" t="s">
-        <v>123</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="L12" s="8">
-        <v>50</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="5"/>
-      <c r="O12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="38" t="s">
+    </row>
+    <row r="32" spans="1:12" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="H32" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="E13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" t="s">
-        <v>125</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="8">
-        <v>5</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="E14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="9">
-        <f>(F11*F12/100)+F13</f>
-        <v>1.6E-2</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" t="s">
-        <v>126</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="8">
-        <f>L10*L13/100</f>
-        <v>0.1</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="5"/>
-      <c r="O14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E15" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="9">
-        <f>F14*1</f>
-        <v>1.6E-2</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I15" t="s">
-        <v>128</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="L15" s="8">
-        <f>L14/0.8</f>
-        <v>0.125</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="5"/>
-      <c r="O15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E16" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="12">
-        <f>F9/(F15*1000)</f>
-        <v>162.5</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" t="s">
-        <v>132</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="L16" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="5"/>
-      <c r="O16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E17" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="12">
-        <f>F10/(F15*1000)</f>
-        <v>68.75</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I17" t="s">
-        <v>133</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L17" s="9">
-        <f>L15+L16</f>
-        <v>0.155</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="5"/>
-      <c r="O17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E18" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="K18" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="L18" s="9">
-        <f>L17*1</f>
-        <v>0.155</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="N18" s="5"/>
-      <c r="O18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="K19" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="L19" s="12">
-        <f>L9/(L18*1000)</f>
-        <v>16.774193548387096</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E20" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="K20" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-    </row>
-    <row r="21" spans="4:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F21" s="8">
-        <v>950</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E22" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F22" s="8">
-        <v>1430</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I22" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D23" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F23" s="8">
-        <v>2750</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E24" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="8">
-        <v>5</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E26" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="9">
-        <f>(F24*F25/100)+F26</f>
-        <v>1.7500000000000002E-2</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E28" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F28" s="9">
-        <f>F27*1</f>
-        <v>1.7500000000000002E-2</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E29" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F29" s="12">
-        <f>F21/(F28*1000)</f>
-        <v>54.285714285714285</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E30" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="12">
-        <f>F22/(F28*1000)</f>
-        <v>81.714285714285708</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I30" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="E31" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" s="12">
-        <f>F23/(F28*1000)</f>
-        <v>157.14285714285714</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="4:15" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E32" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+    </row>
+    <row r="33" spans="8:12" x14ac:dyDescent="0.35">
+      <c r="H33" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>